<commit_message>
align with master create db
</commit_message>
<xml_diff>
--- a/data/mosad.xlsx
+++ b/data/mosad.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OZKL\T_H\backflask---T.H-app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE7D7743-1D4A-4A5A-B7CB-6694FA068B7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{630D5B59-603C-4AF6-9E84-8D99634DF843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="1060" windowWidth="14400" windowHeight="7510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="מספרים ייחודים" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
   <si>
     <t>עלי</t>
   </si>
@@ -99,9 +99,6 @@
     <t>בני דוד הבקעה</t>
   </si>
   <si>
-    <t>בני דוד</t>
-  </si>
-  <si>
     <t>eldad8797@gmail.com</t>
   </si>
   <si>
@@ -126,7 +123,10 @@
     <t>contact_name</t>
   </si>
   <si>
-    <t>לא ידוע</t>
+    <t>מרכז</t>
+  </si>
+  <si>
+    <t>דרום</t>
   </si>
 </sst>
 </file>
@@ -471,13 +471,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:W5"/>
+  <dimension ref="A1:W4"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomRight" activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -543,10 +543,10 @@
         <v>4</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
@@ -566,22 +566,22 @@
         <v>543124511</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="E2" s="8">
         <v>543124511</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G2" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="9" t="s">
         <v>20</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>21</v>
       </c>
       <c r="I2" s="10">
         <v>543124517</v>
@@ -594,7 +594,7 @@
         <v>0</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N2" s="8">
         <v>543124511</v>
@@ -608,22 +608,22 @@
         <v>543124512</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="E3" s="8">
         <v>543124512</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I3" s="8">
         <v>543124512</v>
@@ -632,10 +632,10 @@
         <v>2</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N3" s="8">
         <v>543124512</v>
@@ -649,22 +649,22 @@
         <v>544817648</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="E4" s="8">
         <v>544817648</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I4" s="10">
         <v>543124511</v>
@@ -673,53 +673,12 @@
         <v>3</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M4" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N4" s="8">
-        <v>544817648</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="8">
-        <v>544817648</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="8">
-        <v>544817648</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5" s="10">
-        <v>543124511</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="M5" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="N5" s="8">
         <v>544817648</v>
       </c>
     </row>

</xml_diff>